<commit_message>
Lagt til HF-kortnavn IndBeskr Høy/Lav->1/0
</commit_message>
<xml_diff>
--- a/data-raw/Indikatorbeskrivelser.xlsx
+++ b/data-raw/Indikatorbeskrivelser.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\SKDE\Nasjonalt servicemiljø\Resultattjenester\Sykehusviser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKDEinterakt\qmongrdata\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Indikatorbeskrivelser" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Indikatorbeskrivelser!$A$1:$I$57</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="259">
   <si>
     <t>IndID</t>
   </si>
@@ -58,9 +61,6 @@
   </si>
   <si>
     <t>KomplSvelging3mnd</t>
-  </si>
-  <si>
-    <t>lav</t>
   </si>
   <si>
     <t xml:space="preserve">Ubehag ved svelging av mat og drikke etter fremre nakkekirurgi (hudåpning på halsen), , ikke-myelopati. </t>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>NDIendr12mnd35pstKI</t>
-  </si>
-  <si>
-    <t>hoy</t>
   </si>
   <si>
     <t>NDI-endring, 12 måneder etter fremre nakkekirurgi (hudåpning på halsen).</t>
@@ -251,9 +248,6 @@
   </si>
   <si>
     <t>ind1_50pstlekkasjeredusjon</t>
-  </si>
-  <si>
-    <t>høy</t>
   </si>
   <si>
     <t xml:space="preserve">Andel pasienter med ? 50% reduksjon av lekkasje i testperiode. </t>
@@ -1640,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,1300 +1682,1300 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E2">
-        <v>0.17</v>
+        <v>0.04</v>
       </c>
       <c r="F2">
-        <v>0.17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
+        <v>0.04</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>0.1</v>
-      </c>
-      <c r="F3">
-        <v>0.1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
+        <v>37</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>0.02</v>
+        <v>0.17</v>
       </c>
       <c r="F4">
-        <v>0.02</v>
-      </c>
-      <c r="G4" t="s">
+        <v>0.17</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
-        <v>0.7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
+        <v>0.1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E6">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="F6">
-        <v>0.04</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
+        <v>0.02</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>0.7</v>
+      </c>
+      <c r="F7">
+        <v>0.7</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>46</v>
+        <v>159</v>
+      </c>
+      <c r="E8">
+        <v>0.8</v>
+      </c>
+      <c r="F8">
+        <v>0.8</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I8" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>50</v>
+        <v>164</v>
+      </c>
+      <c r="E9">
+        <v>0.7</v>
+      </c>
+      <c r="F9">
+        <v>0.7</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>165</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>55</v>
+        <v>169</v>
+      </c>
+      <c r="E10">
+        <v>0.4</v>
+      </c>
+      <c r="F10">
+        <v>0.4</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>165</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>171</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>60</v>
+        <v>172</v>
+      </c>
+      <c r="E11">
+        <v>0.9</v>
+      </c>
+      <c r="F11">
+        <v>0.9</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>165</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>65</v>
+        <v>175</v>
+      </c>
+      <c r="E12">
+        <v>0.8</v>
+      </c>
+      <c r="F12">
+        <v>0.8</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>176</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>65</v>
+        <v>180</v>
+      </c>
+      <c r="E13">
+        <v>0.9</v>
+      </c>
+      <c r="F13">
+        <v>0.9</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>181</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>221</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>222</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>223</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="E14">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="F14">
-        <v>0.7</v>
-      </c>
-      <c r="G14" t="s">
-        <v>74</v>
+        <v>0.3</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>227</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>222</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>228</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>229</v>
       </c>
       <c r="E15">
-        <v>0.95</v>
+        <v>0.3</v>
       </c>
       <c r="F15">
-        <v>0.95</v>
-      </c>
-      <c r="G15" t="s">
-        <v>74</v>
+        <v>0.25</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>80</v>
+        <v>230</v>
       </c>
       <c r="I15" t="s">
-        <v>81</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>222</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>233</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>234</v>
       </c>
       <c r="E16">
-        <v>0.04</v>
+        <v>0.5</v>
       </c>
       <c r="F16">
-        <v>0.04</v>
-      </c>
-      <c r="G16" t="s">
-        <v>13</v>
+        <v>0.4</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>85</v>
+        <v>233</v>
       </c>
       <c r="I16" t="s">
-        <v>86</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>236</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>222</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>237</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>238</v>
       </c>
       <c r="E17">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="F17">
-        <v>0.3</v>
-      </c>
-      <c r="G17" t="s">
-        <v>74</v>
+        <v>0.4</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>91</v>
+        <v>239</v>
+      </c>
+      <c r="I17" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>222</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>242</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="E18">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="F18">
-        <v>0.3</v>
-      </c>
-      <c r="G18" t="s">
-        <v>74</v>
+        <v>0.4</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>94</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>95</v>
+        <v>239</v>
+      </c>
+      <c r="I18" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>222</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>245</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>246</v>
       </c>
       <c r="E19">
         <v>0.5</v>
       </c>
       <c r="F19">
-        <v>0.5</v>
-      </c>
-      <c r="G19" t="s">
-        <v>74</v>
+        <v>0.4</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>91</v>
+        <v>247</v>
+      </c>
+      <c r="I19" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>249</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>222</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>250</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>251</v>
       </c>
       <c r="E20">
         <v>0.5</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
-      </c>
-      <c r="G20" t="s">
-        <v>74</v>
+        <v>0.4</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>102</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="I20" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>254</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>255</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>256</v>
       </c>
       <c r="E21">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F21">
-        <v>0.3</v>
-      </c>
-      <c r="G21" t="s">
-        <v>74</v>
+        <v>0.1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>90</v>
+        <v>257</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>91</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>185</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>186</v>
       </c>
       <c r="E22">
-        <v>0.3</v>
+        <v>0.03</v>
       </c>
       <c r="F22">
-        <v>0.3</v>
-      </c>
-      <c r="G22" t="s">
-        <v>74</v>
+        <v>0.04</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>108</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>91</v>
+        <v>187</v>
+      </c>
+      <c r="I22" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>218</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>184</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>219</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>220</v>
       </c>
       <c r="E23">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
-      </c>
-      <c r="G23" t="s">
-        <v>74</v>
+        <v>0.6</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>91</v>
+        <v>213</v>
+      </c>
+      <c r="I23" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>189</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
+        <v>191</v>
       </c>
       <c r="E24">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="F24">
-        <v>0.5</v>
-      </c>
-      <c r="G24" t="s">
-        <v>74</v>
+        <v>0.08</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>114</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>184</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
-        <v>117</v>
+        <v>195</v>
       </c>
       <c r="E25">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="F25">
-        <v>0.3</v>
-      </c>
-      <c r="G25" t="s">
-        <v>74</v>
+        <v>0.08</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>118</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
+        <v>197</v>
       </c>
       <c r="D26" t="s">
-        <v>121</v>
+        <v>198</v>
       </c>
       <c r="E26">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="F26">
-        <v>0.5</v>
-      </c>
-      <c r="G26" t="s">
-        <v>74</v>
+        <v>0.08</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>200</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>201</v>
       </c>
       <c r="E27">
-        <v>0.94</v>
+        <v>0.03</v>
       </c>
       <c r="F27">
-        <v>0.94</v>
-      </c>
-      <c r="G27" t="s">
-        <v>74</v>
+        <v>0.05</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>127</v>
-      </c>
-      <c r="I27" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>203</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
       <c r="E28">
-        <v>0.79</v>
+        <v>0.04</v>
       </c>
       <c r="F28">
-        <v>0.79</v>
-      </c>
-      <c r="G28" t="s">
-        <v>74</v>
+        <v>0.06</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>132</v>
+        <v>205</v>
       </c>
       <c r="I28" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="C29" t="s">
-        <v>135</v>
+        <v>208</v>
       </c>
       <c r="D29" t="s">
-        <v>136</v>
+        <v>209</v>
       </c>
       <c r="E29">
-        <v>0.94</v>
+        <v>0.05</v>
       </c>
       <c r="F29">
-        <v>0.94</v>
-      </c>
-      <c r="G29" t="s">
-        <v>74</v>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>137</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>138</v>
+        <v>205</v>
+      </c>
+      <c r="I29" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>210</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="C30" t="s">
-        <v>140</v>
+        <v>211</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>212</v>
       </c>
       <c r="E30">
-        <v>0.79</v>
+        <v>0.3</v>
       </c>
       <c r="F30">
-        <v>0.79</v>
-      </c>
-      <c r="G30" t="s">
-        <v>74</v>
+        <v>0.3</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>142</v>
+        <v>213</v>
       </c>
       <c r="I30" t="s">
-        <v>143</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>216</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>217</v>
       </c>
       <c r="E31">
-        <v>0.79</v>
+        <v>0.7</v>
       </c>
       <c r="F31">
-        <v>0.79</v>
-      </c>
-      <c r="G31" t="s">
-        <v>74</v>
+        <v>0.6</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>147</v>
+        <v>213</v>
       </c>
       <c r="I31" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32">
+        <v>0.94</v>
+      </c>
+      <c r="F32">
+        <v>0.94</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
         <v>124</v>
       </c>
-      <c r="C32" t="s">
-        <v>150</v>
-      </c>
-      <c r="D32" t="s">
-        <v>151</v>
-      </c>
-      <c r="E32">
-        <v>0.59</v>
-      </c>
-      <c r="F32">
-        <v>0.59</v>
-      </c>
-      <c r="G32" t="s">
-        <v>74</v>
-      </c>
-      <c r="H32" t="s">
-        <v>152</v>
-      </c>
       <c r="I32" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="E33">
-        <v>0.59</v>
+        <v>0.79</v>
       </c>
       <c r="F33">
-        <v>0.59</v>
-      </c>
-      <c r="G33" t="s">
-        <v>74</v>
+        <v>0.79</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="I33" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="B34" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="D34" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="E34">
-        <v>0.8</v>
+        <v>0.94</v>
       </c>
       <c r="F34">
-        <v>0.8</v>
+        <v>0.94</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>163</v>
-      </c>
-      <c r="I34" t="s">
-        <v>164</v>
+        <v>134</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="C35" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="D35" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="E35">
-        <v>0.7</v>
+        <v>0.79</v>
       </c>
       <c r="F35">
-        <v>0.7</v>
+        <v>0.79</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="I35" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="C36" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="E36">
-        <v>0.4</v>
+        <v>0.79</v>
       </c>
       <c r="F36">
-        <v>0.4</v>
+        <v>0.79</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="I36" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="D37" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="E37">
-        <v>0.9</v>
+        <v>0.59</v>
       </c>
       <c r="F37">
-        <v>0.9</v>
+        <v>0.59</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="I37" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="C38" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="D38" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="E38">
-        <v>0.8</v>
+        <v>0.59</v>
       </c>
       <c r="F38">
-        <v>0.8</v>
+        <v>0.59</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="I38" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>182</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>183</v>
+        <v>71</v>
       </c>
       <c r="E39">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="F39">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>184</v>
+        <v>72</v>
       </c>
       <c r="I39" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>186</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>187</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>188</v>
+        <v>107</v>
       </c>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>108</v>
       </c>
       <c r="E40">
-        <v>0.03</v>
+        <v>0.5</v>
       </c>
       <c r="F40">
-        <v>0.04</v>
-      </c>
-      <c r="G40" t="s">
-        <v>13</v>
+        <v>0.5</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>190</v>
-      </c>
-      <c r="I40" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>192</v>
+        <v>68</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>193</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s">
-        <v>194</v>
+        <v>110</v>
       </c>
       <c r="E41">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="F41">
-        <v>0.08</v>
-      </c>
-      <c r="G41" t="s">
-        <v>13</v>
+        <v>0.5</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>187</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>197</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>198</v>
+        <v>114</v>
       </c>
       <c r="E42">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="F42">
-        <v>0.08</v>
-      </c>
-      <c r="G42" t="s">
-        <v>13</v>
+        <v>0.3</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="C43" t="s">
-        <v>200</v>
+        <v>117</v>
       </c>
       <c r="D43" t="s">
-        <v>201</v>
+        <v>118</v>
       </c>
       <c r="E43">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="F43">
-        <v>0.08</v>
-      </c>
-      <c r="G43" t="s">
-        <v>13</v>
+        <v>0.5</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>195</v>
+        <v>119</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>202</v>
+        <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>187</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
-        <v>203</v>
+        <v>75</v>
       </c>
       <c r="D44" t="s">
-        <v>204</v>
+        <v>76</v>
       </c>
       <c r="E44">
-        <v>0.03</v>
+        <v>0.95</v>
       </c>
       <c r="F44">
-        <v>0.05</v>
-      </c>
-      <c r="G44" t="s">
-        <v>13</v>
+        <v>0.95</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>195</v>
+        <v>77</v>
+      </c>
+      <c r="I44" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>206</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>207</v>
+        <v>81</v>
       </c>
       <c r="E45">
         <v>0.04</v>
       </c>
       <c r="F45">
-        <v>0.06</v>
-      </c>
-      <c r="G45" t="s">
-        <v>13</v>
+        <v>0.04</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>208</v>
+        <v>82</v>
       </c>
       <c r="I45" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>210</v>
+        <v>68</v>
       </c>
       <c r="B46" t="s">
-        <v>187</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>211</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
-        <v>212</v>
+        <v>86</v>
       </c>
       <c r="E46">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="F46">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G46" t="s">
-        <v>13</v>
+        <v>0.3</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>208</v>
-      </c>
-      <c r="I46" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>213</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>187</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>214</v>
+        <v>85</v>
       </c>
       <c r="D47" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="E47">
         <v>0.3</v>
@@ -2989,86 +2983,86 @@
       <c r="F47">
         <v>0.3</v>
       </c>
-      <c r="G47" t="s">
-        <v>74</v>
+      <c r="G47">
+        <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>216</v>
-      </c>
-      <c r="I47" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>218</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>187</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>219</v>
+        <v>94</v>
       </c>
       <c r="D48" t="s">
-        <v>220</v>
+        <v>95</v>
       </c>
       <c r="E48">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="F48">
-        <v>0.6</v>
-      </c>
-      <c r="G48" t="s">
-        <v>74</v>
+        <v>0.5</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I48" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>221</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>222</v>
+        <v>94</v>
       </c>
       <c r="D49" t="s">
-        <v>223</v>
+        <v>98</v>
       </c>
       <c r="E49">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="F49">
-        <v>0.6</v>
-      </c>
-      <c r="G49" t="s">
-        <v>74</v>
+        <v>0.5</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>216</v>
-      </c>
-      <c r="I49" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>225</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
-        <v>226</v>
+        <v>101</v>
       </c>
       <c r="D50" t="s">
-        <v>227</v>
+        <v>102</v>
       </c>
       <c r="E50">
         <v>0.3</v>
@@ -3076,217 +3070,217 @@
       <c r="F50">
         <v>0.3</v>
       </c>
-      <c r="G50" t="s">
-        <v>74</v>
+      <c r="G50">
+        <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>228</v>
-      </c>
-      <c r="I50" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>230</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
-        <v>225</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>231</v>
+        <v>101</v>
       </c>
       <c r="D51" t="s">
-        <v>232</v>
+        <v>104</v>
       </c>
       <c r="E51">
         <v>0.3</v>
       </c>
       <c r="F51">
-        <v>0.25</v>
-      </c>
-      <c r="G51" t="s">
-        <v>74</v>
+        <v>0.3</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>233</v>
-      </c>
-      <c r="I51" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>235</v>
+        <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="C52" t="s">
-        <v>236</v>
+        <v>41</v>
       </c>
       <c r="D52" t="s">
-        <v>237</v>
-      </c>
-      <c r="E52">
-        <v>0.5</v>
-      </c>
-      <c r="F52">
-        <v>0.4</v>
-      </c>
-      <c r="G52" t="s">
-        <v>74</v>
-      </c>
-      <c r="H52" t="s">
-        <v>236</v>
-      </c>
-      <c r="I52" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>239</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>240</v>
+        <v>46</v>
       </c>
       <c r="D53" t="s">
-        <v>241</v>
-      </c>
-      <c r="E53">
-        <v>0.5</v>
-      </c>
-      <c r="F53">
-        <v>0.4</v>
-      </c>
-      <c r="G53" t="s">
-        <v>74</v>
-      </c>
-      <c r="H53" t="s">
-        <v>242</v>
+        <v>47</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="I53" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>244</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>245</v>
+        <v>51</v>
       </c>
       <c r="D54" t="s">
-        <v>246</v>
-      </c>
-      <c r="E54">
-        <v>0.5</v>
-      </c>
-      <c r="F54">
-        <v>0.4</v>
-      </c>
-      <c r="G54" t="s">
-        <v>74</v>
-      </c>
-      <c r="H54" t="s">
-        <v>242</v>
+        <v>52</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="I54" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>247</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>248</v>
+        <v>56</v>
       </c>
       <c r="D55" t="s">
-        <v>249</v>
-      </c>
-      <c r="E55">
-        <v>0.5</v>
-      </c>
-      <c r="F55">
-        <v>0.4</v>
-      </c>
-      <c r="G55" t="s">
-        <v>74</v>
-      </c>
-      <c r="H55" t="s">
-        <v>250</v>
+        <v>57</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="I55" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>252</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>253</v>
+        <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>254</v>
-      </c>
-      <c r="E56">
-        <v>0.5</v>
-      </c>
-      <c r="F56">
-        <v>0.4</v>
-      </c>
-      <c r="G56" t="s">
-        <v>74</v>
-      </c>
-      <c r="H56" t="s">
-        <v>255</v>
+        <v>62</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="I56" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>257</v>
+        <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>258</v>
+        <v>66</v>
       </c>
       <c r="D57" t="s">
-        <v>259</v>
-      </c>
-      <c r="E57">
-        <v>0.1</v>
-      </c>
-      <c r="F57">
-        <v>0.1</v>
-      </c>
-      <c r="G57" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" t="s">
-        <v>260</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>261</v>
+        <v>67</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I57" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Lastoppdata (#13)" (#16)
* Revert "Lastoppdata (#13)"

This reverts commit 509ae4c3a29c3f682084f0bfe262e981b60912a9.

* revert data-raw/tilretteleggKvalIndData.R to master version
</commit_message>
<xml_diff>
--- a/data-raw/Indikatorbeskrivelser.xlsx
+++ b/data-raw/Indikatorbeskrivelser.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\qmongrdata\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKDEinterakt\qmongrdata\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1634,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2734,10 +2734,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" t="s">
         <v>69</v>
-      </c>
-      <c r="B39" t="s">
-        <v>68</v>
       </c>
       <c r="C39" t="s">
         <v>70</v>
@@ -2763,10 +2763,10 @@
     </row>
     <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" t="s">
         <v>106</v>
-      </c>
-      <c r="B40" t="s">
-        <v>68</v>
       </c>
       <c r="C40" t="s">
         <v>107</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
         <v>109</v>
-      </c>
-      <c r="B41" t="s">
-        <v>68</v>
       </c>
       <c r="C41" t="s">
         <v>107</v>
@@ -2821,10 +2821,10 @@
     </row>
     <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" t="s">
         <v>112</v>
-      </c>
-      <c r="B42" t="s">
-        <v>68</v>
       </c>
       <c r="C42" t="s">
         <v>113</v>
@@ -2850,10 +2850,10 @@
     </row>
     <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" t="s">
         <v>116</v>
-      </c>
-      <c r="B43" t="s">
-        <v>68</v>
       </c>
       <c r="C43" t="s">
         <v>117</v>
@@ -2879,10 +2879,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" t="s">
         <v>74</v>
-      </c>
-      <c r="B44" t="s">
-        <v>68</v>
       </c>
       <c r="C44" t="s">
         <v>75</v>
@@ -2908,10 +2908,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
         <v>79</v>
-      </c>
-      <c r="B45" t="s">
-        <v>68</v>
       </c>
       <c r="C45" t="s">
         <v>80</v>
@@ -2937,10 +2937,10 @@
     </row>
     <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" t="s">
         <v>84</v>
-      </c>
-      <c r="B46" t="s">
-        <v>68</v>
       </c>
       <c r="C46" t="s">
         <v>85</v>
@@ -2966,10 +2966,10 @@
     </row>
     <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" t="s">
         <v>89</v>
-      </c>
-      <c r="B47" t="s">
-        <v>68</v>
       </c>
       <c r="C47" t="s">
         <v>85</v>
@@ -2995,10 +2995,10 @@
     </row>
     <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
         <v>93</v>
-      </c>
-      <c r="B48" t="s">
-        <v>68</v>
       </c>
       <c r="C48" t="s">
         <v>94</v>
@@ -3024,10 +3024,10 @@
     </row>
     <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s">
         <v>97</v>
-      </c>
-      <c r="B49" t="s">
-        <v>68</v>
       </c>
       <c r="C49" t="s">
         <v>94</v>
@@ -3053,10 +3053,10 @@
     </row>
     <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" t="s">
         <v>100</v>
-      </c>
-      <c r="B50" t="s">
-        <v>68</v>
       </c>
       <c r="C50" t="s">
         <v>101</v>
@@ -3082,10 +3082,10 @@
     </row>
     <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" t="s">
         <v>103</v>
-      </c>
-      <c r="B51" t="s">
-        <v>68</v>
       </c>
       <c r="C51" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Fix mistake in IndBeskr data
IndID and Register were swapped for nra
</commit_message>
<xml_diff>
--- a/data-raw/Indikatorbeskrivelser.xlsx
+++ b/data-raw/Indikatorbeskrivelser.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKDEinterakt\qmongrdata\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnfinn/repo/qmongrdata/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BD2B63-833A-3449-89F1-D891E74FBFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14175"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indikatorbeskrivelser" sheetId="1" r:id="rId1"/>
@@ -827,7 +828,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1313,48 +1314,48 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Dårlig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="God" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Inndata" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Koblet celle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Kontrollcelle" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Merknad" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nøytral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Tittel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totalt" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Varseltekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1631,27 +1632,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="199.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="199.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>162</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>170</v>
       </c>
@@ -1961,7 +1962,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -1990,7 +1991,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>221</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>227</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>232</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>241</v>
       </c>
@@ -2164,7 +2165,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>244</v>
       </c>
@@ -2193,7 +2194,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>249</v>
       </c>
@@ -2222,7 +2223,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>183</v>
       </c>
@@ -2280,7 +2281,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>218</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>189</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>193</v>
       </c>
@@ -2361,7 +2362,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>199</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>202</v>
       </c>
@@ -2442,7 +2443,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>207</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>210</v>
       </c>
@@ -2500,7 +2501,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -2587,7 +2588,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -2674,7 +2675,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>146</v>
       </c>
@@ -2703,7 +2704,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -2732,12 +2733,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
         <v>68</v>
-      </c>
-      <c r="B39" t="s">
-        <v>69</v>
       </c>
       <c r="C39" t="s">
         <v>70</v>
@@ -2761,12 +2762,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" t="s">
         <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>106</v>
       </c>
       <c r="C40" t="s">
         <v>107</v>
@@ -2790,12 +2791,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" t="s">
         <v>68</v>
-      </c>
-      <c r="B41" t="s">
-        <v>109</v>
       </c>
       <c r="C41" t="s">
         <v>107</v>
@@ -2819,12 +2820,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
         <v>68</v>
-      </c>
-      <c r="B42" t="s">
-        <v>112</v>
       </c>
       <c r="C42" t="s">
         <v>113</v>
@@ -2848,12 +2849,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" t="s">
         <v>68</v>
-      </c>
-      <c r="B43" t="s">
-        <v>116</v>
       </c>
       <c r="C43" t="s">
         <v>117</v>
@@ -2877,12 +2878,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
         <v>68</v>
-      </c>
-      <c r="B44" t="s">
-        <v>74</v>
       </c>
       <c r="C44" t="s">
         <v>75</v>
@@ -2906,12 +2907,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
         <v>68</v>
-      </c>
-      <c r="B45" t="s">
-        <v>79</v>
       </c>
       <c r="C45" t="s">
         <v>80</v>
@@ -2935,12 +2936,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
         <v>68</v>
-      </c>
-      <c r="B46" t="s">
-        <v>84</v>
       </c>
       <c r="C46" t="s">
         <v>85</v>
@@ -2964,12 +2965,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" t="s">
         <v>68</v>
-      </c>
-      <c r="B47" t="s">
-        <v>89</v>
       </c>
       <c r="C47" t="s">
         <v>85</v>
@@ -2993,12 +2994,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
         <v>68</v>
-      </c>
-      <c r="B48" t="s">
-        <v>93</v>
       </c>
       <c r="C48" t="s">
         <v>94</v>
@@ -3022,12 +3023,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
         <v>68</v>
-      </c>
-      <c r="B49" t="s">
-        <v>97</v>
       </c>
       <c r="C49" t="s">
         <v>94</v>
@@ -3051,12 +3052,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
         <v>68</v>
-      </c>
-      <c r="B50" t="s">
-        <v>100</v>
       </c>
       <c r="C50" t="s">
         <v>101</v>
@@ -3080,12 +3081,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
         <v>68</v>
-      </c>
-      <c r="B51" t="s">
-        <v>103</v>
       </c>
       <c r="C51" t="s">
         <v>101</v>
@@ -3109,7 +3110,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -3138,7 +3139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -3167,7 +3168,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -3225,7 +3226,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -3254,7 +3255,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Fix mistake in IndBeskr data. (#17)
IndID and Register were swapped for nra
</commit_message>
<xml_diff>
--- a/data-raw/Indikatorbeskrivelser.xlsx
+++ b/data-raw/Indikatorbeskrivelser.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKDEinterakt\qmongrdata\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnfinn/repo/qmongrdata/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BD2B63-833A-3449-89F1-D891E74FBFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14175"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indikatorbeskrivelser" sheetId="1" r:id="rId1"/>
@@ -827,7 +828,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1313,48 +1314,48 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Dårlig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="God" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Inndata" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Koblet celle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Kontrollcelle" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Merknad" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nøytral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Tittel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totalt" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Varseltekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1631,27 +1632,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="199.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="199.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>162</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>170</v>
       </c>
@@ -1961,7 +1962,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -1990,7 +1991,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>221</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>227</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>232</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>241</v>
       </c>
@@ -2164,7 +2165,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>244</v>
       </c>
@@ -2193,7 +2194,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>249</v>
       </c>
@@ -2222,7 +2223,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>183</v>
       </c>
@@ -2280,7 +2281,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>218</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>189</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>193</v>
       </c>
@@ -2361,7 +2362,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>199</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>202</v>
       </c>
@@ -2442,7 +2443,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>207</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>210</v>
       </c>
@@ -2500,7 +2501,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -2587,7 +2588,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -2674,7 +2675,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>146</v>
       </c>
@@ -2703,7 +2704,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -2732,12 +2733,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
         <v>68</v>
-      </c>
-      <c r="B39" t="s">
-        <v>69</v>
       </c>
       <c r="C39" t="s">
         <v>70</v>
@@ -2761,12 +2762,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" t="s">
         <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>106</v>
       </c>
       <c r="C40" t="s">
         <v>107</v>
@@ -2790,12 +2791,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" t="s">
         <v>68</v>
-      </c>
-      <c r="B41" t="s">
-        <v>109</v>
       </c>
       <c r="C41" t="s">
         <v>107</v>
@@ -2819,12 +2820,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
         <v>68</v>
-      </c>
-      <c r="B42" t="s">
-        <v>112</v>
       </c>
       <c r="C42" t="s">
         <v>113</v>
@@ -2848,12 +2849,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" t="s">
         <v>68</v>
-      </c>
-      <c r="B43" t="s">
-        <v>116</v>
       </c>
       <c r="C43" t="s">
         <v>117</v>
@@ -2877,12 +2878,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
         <v>68</v>
-      </c>
-      <c r="B44" t="s">
-        <v>74</v>
       </c>
       <c r="C44" t="s">
         <v>75</v>
@@ -2906,12 +2907,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
         <v>68</v>
-      </c>
-      <c r="B45" t="s">
-        <v>79</v>
       </c>
       <c r="C45" t="s">
         <v>80</v>
@@ -2935,12 +2936,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
         <v>68</v>
-      </c>
-      <c r="B46" t="s">
-        <v>84</v>
       </c>
       <c r="C46" t="s">
         <v>85</v>
@@ -2964,12 +2965,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" t="s">
         <v>68</v>
-      </c>
-      <c r="B47" t="s">
-        <v>89</v>
       </c>
       <c r="C47" t="s">
         <v>85</v>
@@ -2993,12 +2994,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
         <v>68</v>
-      </c>
-      <c r="B48" t="s">
-        <v>93</v>
       </c>
       <c r="C48" t="s">
         <v>94</v>
@@ -3022,12 +3023,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
         <v>68</v>
-      </c>
-      <c r="B49" t="s">
-        <v>97</v>
       </c>
       <c r="C49" t="s">
         <v>94</v>
@@ -3051,12 +3052,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
         <v>68</v>
-      </c>
-      <c r="B50" t="s">
-        <v>100</v>
       </c>
       <c r="C50" t="s">
         <v>101</v>
@@ -3080,12 +3081,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
         <v>68</v>
-      </c>
-      <c r="B51" t="s">
-        <v>103</v>
       </c>
       <c r="C51" t="s">
         <v>101</v>
@@ -3109,7 +3110,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -3138,7 +3139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -3167,7 +3168,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -3225,7 +3226,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -3254,7 +3255,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Update IndBeskr, hjerteinfarkt and lymfoid
</commit_message>
<xml_diff>
--- a/data-raw/Indikatorbeskrivelser.xlsx
+++ b/data-raw/Indikatorbeskrivelser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnfinn/repo/qmongrdata/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\repo\qmongrdata\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F77EB8-C1E7-AB49-BF9B-85DE7ED27D51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E8969A-BB45-471B-AE3D-A423A04E1391}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indikatorbeskrivelser" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Indikatorbeskrivelser!$A$1:$I$57</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="375">
   <si>
     <t>IndID</t>
   </si>
@@ -950,12 +950,283 @@
   <si>
     <t>hoftebrudd</t>
   </si>
+  <si>
+    <t>lymfoid1</t>
+  </si>
+  <si>
+    <t>lymfoid2</t>
+  </si>
+  <si>
+    <t>lymfoid3</t>
+  </si>
+  <si>
+    <t>lymfoid4</t>
+  </si>
+  <si>
+    <t>lymfoid5</t>
+  </si>
+  <si>
+    <t>lymfoid6</t>
+  </si>
+  <si>
+    <t>lymfoid</t>
+  </si>
+  <si>
+    <t>Dekningsgrad: Utredning</t>
+  </si>
+  <si>
+    <t>Diagnostisering av non-Hodgkin lymfom</t>
+  </si>
+  <si>
+    <t>Angitt stadium v/ non-Hodgkin lymfom</t>
+  </si>
+  <si>
+    <t>Flowcytometri v/ kronisk lymfatisk leukemi</t>
+  </si>
+  <si>
+    <t>Biopsi v/ myelomatose</t>
+  </si>
+  <si>
+    <t>FISH v/ myelomatose</t>
+  </si>
+  <si>
+    <t>kiB</t>
+  </si>
+  <si>
+    <t>kiC</t>
+  </si>
+  <si>
+    <t>kiC1</t>
+  </si>
+  <si>
+    <t>kiC2</t>
+  </si>
+  <si>
+    <t>kiD</t>
+  </si>
+  <si>
+    <t>kiE</t>
+  </si>
+  <si>
+    <t>kiF</t>
+  </si>
+  <si>
+    <t>kiG</t>
+  </si>
+  <si>
+    <t>kiH</t>
+  </si>
+  <si>
+    <t>kiJ</t>
+  </si>
+  <si>
+    <t>kiK</t>
+  </si>
+  <si>
+    <t>kiA</t>
+  </si>
+  <si>
+    <t>Reperfusjonsbehandling ved STEMI</t>
+  </si>
+  <si>
+    <t>Reperfusjonsbehandling innen anbefalt tid ved STEMI</t>
+  </si>
+  <si>
+    <t>Trombolyse innen anbefalt tid</t>
+  </si>
+  <si>
+    <t>Primær PCI innen anbefalt tid</t>
+  </si>
+  <si>
+    <t>Invasivt utredet ved NSTEMI</t>
+  </si>
+  <si>
+    <t>Invasivt utredet innen 72 timer ved NSTEMI</t>
+  </si>
+  <si>
+    <t>Utskrevet med antitrombotisk behandling</t>
+  </si>
+  <si>
+    <t>Utskrevet med lipidsenkende medikament</t>
+  </si>
+  <si>
+    <t>Ejeksjonsfraksjon (EF) målt</t>
+  </si>
+  <si>
+    <t>Utskrevet med betablokker hvis indikasjon</t>
+  </si>
+  <si>
+    <t>ACE-hemmer/AII-antagonist hvis indikasjon</t>
+  </si>
+  <si>
+    <t>Dekningsgrad</t>
+  </si>
+  <si>
+    <t>hjerteinfarkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klinisk utredningsskjema for lymfoide maligniteter er viktig for å vurdere blant annet utbredelse og antatt forløp. </t>
+  </si>
+  <si>
+    <t>I følge både pakkeforløp og handlingsprogram skal alle lymfomdiagnoser stilles etter vurdering ved et universitetssykehuslaboratorium.</t>
+  </si>
+  <si>
+    <t>Stadium viser hvor utbredt sykdommen er og er en viktig prognostisk faktor.</t>
+  </si>
+  <si>
+    <t>Ved diagnostisering av kronisk lymfatisk leukemi anbefales det å bruke undersøkelsen flowcytometri.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handlingsprogrammet anbefaler biopsi som undersøkelsesmetode for fastsetting av myelomatose. </t>
+  </si>
+  <si>
+    <t>Handlingsprogrammet anbefaler FISH som standardmetode for cytogenetisk undersøkelse ved diagnostisering av myelomatose.</t>
+  </si>
+  <si>
+    <t>Figuren viser dekningsgrad av primærutredning for 2018 og 2019. Informasjon om morfologi, basis for diagnosen, diagnosedato, tilhørende sykehus etc. hentes fra patologibesvarelsen der komplettheten ligger på 97,35 prosent. Stadium, prognostiske faktorer og planlagt behandling er derimot informasjon registeret kun får via utredningsmelding og registeret har derfor hatt høy fokus på å forbedre rapporteringen. Høy grad av måloppnåelse for denne kvalitetsindikatoren er 80% eller mer.</t>
+  </si>
+  <si>
+    <t>Figuren viser andelen av pasienter diagnostisert med non-Hodgkin lymfom i 2019 som har fått diagnosen stilt ved et universitetssykehus, eller ved konsultasjon fra et universitetssykehus. Høy grad av måloppnåelse for denne kvalitetsindikatoren er over 95 prosent. Noen pasienter får ikke diagnosen stilt ved hjelp av anbefalt konsultasjon med universitetssykehus med erfaring, kompetanse og nødvendig utstyr for immunhistokjemisk og molekylær lymfomdiagnostikk. Registeret vil se på de ulike årsakene til dette og oppfordrer alle laboratorier til å følge retningslinjene.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figuren viser andelen av pasienter diagnostisert med non-Hodgkin lymfom der stadium er oppgitt på utredningsmeldingen. Å angi riktig stadium er en viktig del av diagnostisering av lymfom. Dette sier noe om hvor utbredt sykdommen er. Høy grad av måloppnåelse for denne kvalitetsindikatoren er 90 prosent eller mer. Målet er nådd med god margin. Resultatet gjelder hele helseforetaket. </t>
+  </si>
+  <si>
+    <t>Flowcytometrisk immunfenotyping er en metode for måling av fysiske og kjemiske egenskaper til enkeltceller eller partikler i væskestrøm, og immunfenotyping av lymfocytter er den anbefalte diagnostiske metoden ved mistanke om kronisk lymfatisk leukemi. Figuren viser andelen av pasienter diagnostisert med kronisk lymfatisk leukemi som har fått diagnosen påvist ved hjelp av flowcytometri fordelt på helseforetak. Høy grad av måloppnåelse for denne kvalitetsindikatoren er 90 prosent eller mer. Resultatet gjelder hele helseforetaket.</t>
+  </si>
+  <si>
+    <t>Figuren viser andelen pasienter diagnostisert med myelomatose i 2019 som er diagnostisert ved hjelp av biopsi (vevsprøve). Resultatet gjelder hele helseforetaket. Praksisen er noe spredt ved de ulike helseforetakene. Biopsi gir sikrere registrering via patologene, sikrere klassifisering ved vanskelig morfologi eller lymfoblastisk fenotype, sikrere tallfesting av plasmacelleandel og vil hos enkelte pasienter gi tidligere behandling. Revidert handlingsprogram for maligne blodsykdommer har endret anbefaling til å benytte seg av biopsi og utstryk, ikke enten/eller.</t>
+  </si>
+  <si>
+    <t>Figuren viser andelen pasienter diagnostisert med myelomatose i 2019 som er diagnostisert ved hjelp av en FISH-analyse. FISH er forkortelse for Fluorescerens In-Situ Hybridisering og er en cytogenetisk teknikk for å detektere og lokalisere tilstedeværelse eller fravær av spesifikke DNA- sekvenser på kromosomer, altså endringer i cellenes molekylære struktur og funksjon. FISH skal være standardmetode for cytogenetisk undersøkelse ved diagnostisering av myelomatose.</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år som ble behandlet med blodpropp-løsende medisin eller utblokking ved mistanke om tett hjerteåre</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år som  i løpet av kort tid ble behandlet med blodpropp-løsende medisin eller utblokking  ved mistanke om tett hjerteåre</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år som  i løpet av kort tid ble behandlet med blodpropp-løsende medisin ved mistanke om tett hjerteåre</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år som i løpet av kort tid ble behandlet med utblokking (PCI)  ved mistanke om tett hjerteåre</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år med mindre EKG-forandringer som ble undersøkt med røntgen av hjertets blodårer i løpet av behandlingsforløpet</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år med mindre EKG-forandringer som ble undersøkt med røntgen av hjertets blodårer innen 72 timer etter innleggelse</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år som behandles med to medikament for å forebygge ny blodpropp etter hjerteinfarktet</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år som behandles med kolesterolsenkende medisin etter hjerteinfarktet</t>
+  </si>
+  <si>
+    <t>Undersøkelse av hjertets pumpefunksjon med ultralyd</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år som fikk anbefalt  medisin (betablokker) for å stabilisere hjerterytmen</t>
+  </si>
+  <si>
+    <t>Pasienter under 85 år med hjertesvikt eller sukkersyke som fikk anbefalt medisin (ACE/AII hemmer)</t>
+  </si>
+  <si>
+    <t>Hvor stor andel av pasienter med hjerteinfarkt som sykehuset meldte til  Norsk hjerteinfarktregister</t>
+  </si>
+  <si>
+    <t>Denne kvalitetsindikatoren er definert som andel pasienter under 85 år som ble behandlet med blodproppløsende medikament eller utblokking ved alvorlig hjerteinfarkt (STEMI). De europeiske retningslinjene som Norsk cardiologisk selskap har sluttet_x000D_
+seg til, anbefaler at pasienter med ST-elevasjonsinfarkt (STEMI) og med &lt;12 timer fra symptomdebut_x000D_
+til første medisinske kontakt (FMK) blir behandlet med trombolyse og/eller koronar angiografi/PCI i_x000D_
+sykdomsforløpet. Hos noen pasienter vil det være medisinsk korrekt å fravike anbefalingene. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t>Kvalitetsindikatoren er definert som andel av pasienter under 85 år som innen anbefalt tid ble behandlet med blodproppløsende medikament eller utblokking ved mistanke om tett hjerteåre og alvorlig hjerteinfarkt (STEMI). Andel pasienter under 85 år innlagt med STelevasjonsinfarkt (STEMI) og med &lt;12 timer fra symptomdebut til første medisinske kontakt som ble_x000D_
+behandlet med trombolyse innen 30 minutter eller koronar angiografi/PCI innen 120 minutter etter_x000D_
+første medisinske kontakt. Ved STEMI skal den tette blodåren åpnes så raskt som overhode mulig._x000D_
+Dette vil gi redusert myokardskade og redusert risiko for hjertesvikt og død. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kvalitetsindikatoren er definert som andel pasienter under 85 år med STEMI som fikk trombolyse_x000D_
+innen 30 minutter av de som ble behandlet med trombolyse som initial reperfusjonsmetode. De europeiske retningslinjene som Norsk cardiologisk selskap har sluttet_x000D_
+seg til, anbefaler at pasienter som har alvorlig hjerteinfarkt med tett hjerteåre får blodproppløsende_x000D_
+medikament innen 30 minutter hvis pasienten ikke kan behandles med utblokking (PCI) innen 120_x000D_
+minutter. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Andel pasienter under 85 år med STEMI og &lt;12 timer fra symptomdebut til første_x000D_
+medisinske kontakt som fikk primær PCI innen 120 minutter etter første medisinske kontakt. Primær_x000D_
+PCI er definert som angiografi eller PCI som initial metode for å oppnå reperfusjon når angiografi_x000D_
+eller PCI ble utført innen 12 timer etter første medisinske kontakt og det ikke var gitt trombolyse på_x000D_
+forhånd. De europeiske retningslinjene som Norsk cardiologisk selskap har sluttet_x000D_
+seg til, anbefaler at pasienter som har alvorlig hjerteinfarkt med tett hjerteåre får behandling med_x000D_
+utblokking (PCI) innen 120 minutter. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t>Kvalitetsindikatoren er definert som andel av pasienter under 85 med mindre EKG-forandringer som ble_x000D_
+undersøkt med røntgen av hjertets blodårer i løpet av behandlingskjeden. De europeiske retningslinjene som Norsk cardiologisk selskap har sluttet_x000D_
+seg til, anbefaler at pasienter med NSTEMI som hovedregel utredes invasivt med koronar angiografi_x000D_
+under sykehusoppholdet. Ved invasiv utredning kartlegges sykdomsutbredelse. Dette er av betydning_x000D_
+for risikostratifisering og planlegging av behandlingen. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t>Kvalitetsindikatoren er definert som andel pasienter under 85 år med mindre EKG-forandringer som ble_x000D_
+undersøkt med røntgen av hjertets blodårer innen 72 timer etter innleggelse. Europeiske retningslinjer anbefaler at pasienter med NSTEMI som_x000D_
+hovedregel gjennomgår invasiv utredning innen 24 timer etter innleggelse. Praksis varierer i Norge._x000D_
+Fagrådet for Norsk hjerteinfarktregister har vurdert foreliggende data og funnet at det ikke foreligger_x000D_
+god dokumentasjon for at pasienter med NSTEMI som hovedregel bør utredes innen 24 timer._x000D_
+Fagrådet har derfor valgt å opprettholde utredning innen 72 timer etter innleggelse som nasjonal_x000D_
+kvalitetsindikator. Det understrekes at pasientene må risikostratifiseres, og at pasienter med høy_x000D_
+risiko må utredes raskt og noen umiddelbart (innen 2 timer). Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t>Kvalitetsindikatoren er definert som andel av pasienter under 85 år som behandles med to platehemmende medikament eller et platehemmende medikament og et antikoagulasjonsbehandlende medikament etter hjerteinfarktet. Antitrombotisk behandling gir prognostisk gevinst. De europeiske_x000D_
+retningslinjene som Norsk cardiologisk selskap har sluttet seg til, anbefaler at pasientene som_x000D_
+hovedregel behandles i 12 måneder med to medikament for å hindre blodpropp etter_x000D_
+hjerteinfarktet. Hos noen pasienter vil det være medisinsk korrekt å fravike anbefalingene. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kvalitetsindikatoren er definert som andel pasienter under 85 år som behandles med_x000D_
+kolesterolsenkende medikament etter hjerteinfarktet. Kolesterolsenkende behandling gir prognostisk gevinst. De europeiske_x000D_
+retningslinjene som Norsk cardiologisk selskap har sluttet seg til, anbefaler at pasientene som_x000D_
+hovedregel behandles med lipidsenkende medikament på ubestemt tid. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t>Kvalitetsindikatoren er definert som andel pasienter som undersøkes med måling av hjertets_x000D_
+pumpefunksjon. De europeiske retningslinjene som Norsk cardiologisk selskap har sluttet_x000D_
+seg til, anbefaler at ejeksjonsfraksjon (hjertets pumpefunksjon) som hovedregel blir beskrevet og_x000D_
+målt under sykdomsforløpet. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t>Kvalitetsindikatoren er definert som andel pasienter under 85 år som fikk anbefalt betablokker_x000D_
+medikament hvis det var indikasjon for betablokker. De europeiske retningslinjene som Norsk cardiologisk selskap har sluttet_x000D_
+seg til, anbefaler at pasientene med EF &lt;40 %, eller som hadde hjertesvikt i tidligere sykehistorie eller_x000D_
+som fikk hjertesvikt i behandlingskjeden som hovedregel bør behandles med betablokker. Hos noen_x000D_
+pasienter vil det være medisinsk korrekt å fravike anbefalingene. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t>Kvalitetsindikatoren er definert som andel pasienter under 85 år med hjertesvikt eller sukkersyke som_x000D_
+fikk medikament ACE-hemmer eller AII-antagonist. De europeiske retningslinjene som Norsk cardiologisk selskap har sluttet_x000D_
+seg til, anbefaler at pasientene med EF &lt;40 %, eller som har hjertesvikt i tidligere sykehistorie, eller_x000D_
+som fikk hjertesvikt som komplikasjon i behandlingskjeden, eller som har sukkersyke, som_x000D_
+hovedregel behandles med ACE-hemmer/AII-antagonist. Hos noen pasienter vil det være medisinsk_x000D_
+korrekt å fravike anbefalingene. Høyt målnivå er ønskelig.</t>
+  </si>
+  <si>
+    <t>God dekningsgrad er en forutsetning for å vurdere kvaliteten på_x000D_
+hjerteinfarktbehandlingen ved det enkelte sykehus. Ved registrering må sykehusene rapportere_x000D_
+hvem de behandler, hvordan de behandler og hva som oppnås ved behandlingen. På den måten blir_x000D_
+registrering av alle hjerteinfarkt ved et sykehus et nødvendig og viktig verktøy for kvalitetsforbedring,_x000D_
+og en forutsetning for å kunne bedømme alle de andre kvalitetsindikatorene.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1089,6 +1360,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1432,56 +1709,58 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Dårlig" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="God" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Inndata" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Koblet celle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Kontrollcelle" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Merknad" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Nøytral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Tittel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Totalt" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Varseltekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1759,26 +2038,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="199.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="199.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1807,7 +2086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1836,7 +2115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1856,7 +2135,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1885,7 +2164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1914,7 +2193,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1943,7 +2222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1972,7 +2251,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -2001,7 +2280,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>162</v>
       </c>
@@ -2030,7 +2309,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -2059,7 +2338,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>170</v>
       </c>
@@ -2088,7 +2367,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -2117,7 +2396,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -2146,7 +2425,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>221</v>
       </c>
@@ -2175,7 +2454,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>227</v>
       </c>
@@ -2204,7 +2483,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>232</v>
       </c>
@@ -2233,7 +2512,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -2262,7 +2541,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>241</v>
       </c>
@@ -2291,7 +2570,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>244</v>
       </c>
@@ -2320,7 +2599,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>249</v>
       </c>
@@ -2349,7 +2628,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -2378,7 +2657,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>183</v>
       </c>
@@ -2407,7 +2686,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>218</v>
       </c>
@@ -2436,7 +2715,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>189</v>
       </c>
@@ -2462,7 +2741,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>193</v>
       </c>
@@ -2488,7 +2767,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -2514,7 +2793,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>199</v>
       </c>
@@ -2540,7 +2819,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>202</v>
       </c>
@@ -2569,7 +2848,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>207</v>
       </c>
@@ -2598,7 +2877,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>210</v>
       </c>
@@ -2627,7 +2906,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -2656,7 +2935,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -2685,7 +2964,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -2714,7 +2993,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -2743,7 +3022,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -2772,7 +3051,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -2801,7 +3080,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>146</v>
       </c>
@@ -2830,7 +3109,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -2859,7 +3138,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -2888,7 +3167,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -2917,7 +3196,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>109</v>
       </c>
@@ -2946,7 +3225,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>112</v>
       </c>
@@ -2975,7 +3254,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -3004,7 +3283,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -3033,7 +3312,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -3062,7 +3341,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -3091,7 +3370,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -3120,7 +3399,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -3149,7 +3428,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -3178,7 +3457,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -3207,7 +3486,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -3236,7 +3515,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -3265,7 +3544,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -3294,7 +3573,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -3323,7 +3602,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -3352,7 +3631,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -3381,7 +3660,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -3410,7 +3689,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>259</v>
       </c>
@@ -3439,7 +3718,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>260</v>
       </c>
@@ -3468,7 +3747,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>261</v>
       </c>
@@ -3497,7 +3776,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>262</v>
       </c>
@@ -3526,7 +3805,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>263</v>
       </c>
@@ -3555,7 +3834,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>264</v>
       </c>
@@ -3584,7 +3863,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>265</v>
       </c>
@@ -3613,7 +3892,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>266</v>
       </c>
@@ -3642,7 +3921,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>267</v>
       </c>
@@ -3671,7 +3950,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>268</v>
       </c>
@@ -3700,7 +3979,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>269</v>
       </c>
@@ -3727,6 +4006,528 @@
       </c>
       <c r="I68" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>301</v>
+      </c>
+      <c r="B69" t="s">
+        <v>307</v>
+      </c>
+      <c r="C69" t="s">
+        <v>308</v>
+      </c>
+      <c r="D69" t="s">
+        <v>301</v>
+      </c>
+      <c r="E69">
+        <v>0.8</v>
+      </c>
+      <c r="F69">
+        <v>0.6</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>339</v>
+      </c>
+      <c r="I69" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>302</v>
+      </c>
+      <c r="B70" t="s">
+        <v>307</v>
+      </c>
+      <c r="C70" t="s">
+        <v>309</v>
+      </c>
+      <c r="D70" t="s">
+        <v>302</v>
+      </c>
+      <c r="E70">
+        <v>0.95</v>
+      </c>
+      <c r="F70">
+        <v>0.9</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70" t="s">
+        <v>340</v>
+      </c>
+      <c r="I70" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>303</v>
+      </c>
+      <c r="B71" t="s">
+        <v>307</v>
+      </c>
+      <c r="C71" t="s">
+        <v>310</v>
+      </c>
+      <c r="D71" t="s">
+        <v>303</v>
+      </c>
+      <c r="E71">
+        <v>0.9</v>
+      </c>
+      <c r="F71">
+        <v>0.8</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" t="s">
+        <v>341</v>
+      </c>
+      <c r="I71" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>304</v>
+      </c>
+      <c r="B72" t="s">
+        <v>307</v>
+      </c>
+      <c r="C72" t="s">
+        <v>311</v>
+      </c>
+      <c r="D72" t="s">
+        <v>304</v>
+      </c>
+      <c r="E72">
+        <v>0.9</v>
+      </c>
+      <c r="F72">
+        <v>0.8</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>342</v>
+      </c>
+      <c r="I72" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>305</v>
+      </c>
+      <c r="B73" t="s">
+        <v>307</v>
+      </c>
+      <c r="C73" t="s">
+        <v>312</v>
+      </c>
+      <c r="D73" t="s">
+        <v>305</v>
+      </c>
+      <c r="E73">
+        <v>0.9</v>
+      </c>
+      <c r="F73">
+        <v>0.8</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73" t="s">
+        <v>343</v>
+      </c>
+      <c r="I73" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>306</v>
+      </c>
+      <c r="B74" t="s">
+        <v>307</v>
+      </c>
+      <c r="C74" t="s">
+        <v>313</v>
+      </c>
+      <c r="D74" t="s">
+        <v>306</v>
+      </c>
+      <c r="E74">
+        <v>0.85</v>
+      </c>
+      <c r="F74">
+        <v>0.7</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74" t="s">
+        <v>344</v>
+      </c>
+      <c r="I74" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B75" t="s">
+        <v>338</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E75" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F75" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B76" t="s">
+        <v>338</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E76" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B77" t="s">
+        <v>338</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E77" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F77" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B78" t="s">
+        <v>338</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E78" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F78" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B79" t="s">
+        <v>338</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E79" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F79" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B80" t="s">
+        <v>338</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E80" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F80" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B81" t="s">
+        <v>338</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E81" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F81" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B82" t="s">
+        <v>338</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E82" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F82" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B83" t="s">
+        <v>338</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E83" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F83" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B84" t="s">
+        <v>338</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E84" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F84" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B85" t="s">
+        <v>338</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E85" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B86" t="s">
+        <v>338</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E86" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F86" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>